<commit_message>
new input,output compare & modify makefile plot.sh
</commit_message>
<xml_diff>
--- a/samplecode/result/result.xlsx
+++ b/samplecode/result/result.xlsx
@@ -9,19 +9,22 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4130" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4130" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="Iterator" sheetId="3" r:id="rId1"/>
-    <sheet name="Alternative" sheetId="4" r:id="rId2"/>
-    <sheet name="Simple" sheetId="1" r:id="rId3"/>
+    <sheet name="Alternative_line" sheetId="4" r:id="rId1"/>
+    <sheet name="Iterator_line" sheetId="3" r:id="rId2"/>
+    <sheet name="Simple_line" sheetId="1" r:id="rId3"/>
+    <sheet name="Alternative_len" sheetId="7" r:id="rId4"/>
+    <sheet name="Iterator_len" sheetId="9" r:id="rId5"/>
+    <sheet name="Simple_len" sheetId="10" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="67">
   <si>
     <t>sorting time</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -181,6 +184,60 @@
   <si>
     <t>sort/total</t>
     <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>len:100,line:1000</t>
+  </si>
+  <si>
+    <t>len:100,line:5000</t>
+  </si>
+  <si>
+    <t>len:100,line:10000</t>
+  </si>
+  <si>
+    <t>len:100,line:50000</t>
+  </si>
+  <si>
+    <t>len:100,line:100000</t>
+  </si>
+  <si>
+    <t>len:100,line:500000</t>
+  </si>
+  <si>
+    <t>len:500,line:1000</t>
+  </si>
+  <si>
+    <t>len:500,line:5000</t>
+  </si>
+  <si>
+    <t>len:500,line:10000</t>
+  </si>
+  <si>
+    <t>len:500,line:50000</t>
+  </si>
+  <si>
+    <t>len:500,line:100000</t>
+  </si>
+  <si>
+    <t>len:500,line:500000</t>
+  </si>
+  <si>
+    <t>len:1000,line:1000</t>
+  </si>
+  <si>
+    <t>len:1000,line:5000</t>
+  </si>
+  <si>
+    <t>len:1000,line:10000</t>
+  </si>
+  <si>
+    <t>len:1000,line:50000</t>
+  </si>
+  <si>
+    <t>len:1000,line:100000</t>
+  </si>
+  <si>
+    <t>len:1000,line:500000</t>
   </si>
 </sst>
 </file>
@@ -1122,505 +1179,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G19"/>
-  <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="2" max="2" width="19.1796875" customWidth="1"/>
-    <col min="3" max="3" width="17.36328125" customWidth="1"/>
-    <col min="4" max="4" width="17.6328125" customWidth="1"/>
-    <col min="5" max="5" width="17.36328125" customWidth="1"/>
-    <col min="6" max="6" width="18.6328125" customWidth="1"/>
-    <col min="7" max="7" width="15.453125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="B1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="3">
-        <v>0</v>
-      </c>
-      <c r="D2" s="3">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="E2" s="3">
-        <v>0.02</v>
-      </c>
-      <c r="F2" s="4">
-        <f>SUM(C2:E2)</f>
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="G2" s="5">
-        <f>D2/F2</f>
-        <v>0.42857142857142849</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="3">
-        <v>0</v>
-      </c>
-      <c r="D3" s="3">
-        <v>6.7000000000000004E-2</v>
-      </c>
-      <c r="E3" s="3">
-        <v>7.2999999999999995E-2</v>
-      </c>
-      <c r="F3" s="4">
-        <f t="shared" ref="F3:F19" si="0">SUM(C3:E3)</f>
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="G3" s="5">
-        <f t="shared" ref="G3:G19" si="1">D3/F3</f>
-        <v>0.47857142857142854</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A4" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="3">
-        <v>0</v>
-      </c>
-      <c r="D4" s="3">
-        <v>0.17599999999999999</v>
-      </c>
-      <c r="E4" s="3">
-        <v>0.184</v>
-      </c>
-      <c r="F4" s="4">
-        <f t="shared" si="0"/>
-        <v>0.36</v>
-      </c>
-      <c r="G4" s="5">
-        <f t="shared" si="1"/>
-        <v>0.48888888888888887</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="3">
-        <v>0</v>
-      </c>
-      <c r="D5" s="3">
-        <v>0.16200000000000001</v>
-      </c>
-      <c r="E5" s="3">
-        <v>0.17299999999999999</v>
-      </c>
-      <c r="F5" s="4">
-        <f t="shared" si="0"/>
-        <v>0.33499999999999996</v>
-      </c>
-      <c r="G5" s="5">
-        <f t="shared" si="1"/>
-        <v>0.48358208955223886</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A6" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="3">
-        <v>0</v>
-      </c>
-      <c r="D6" s="3">
-        <v>0.44800000000000001</v>
-      </c>
-      <c r="E6" s="3">
-        <v>0.46</v>
-      </c>
-      <c r="F6" s="4">
-        <f t="shared" si="0"/>
-        <v>0.90800000000000003</v>
-      </c>
-      <c r="G6" s="5">
-        <f t="shared" si="1"/>
-        <v>0.4933920704845815</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A7" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="3">
-        <v>0</v>
-      </c>
-      <c r="D7" s="3">
-        <v>1.3879999999999999</v>
-      </c>
-      <c r="E7" s="3">
-        <v>1.3979999999999999</v>
-      </c>
-      <c r="F7" s="4">
-        <f t="shared" si="0"/>
-        <v>2.7859999999999996</v>
-      </c>
-      <c r="G7" s="5">
-        <f t="shared" si="1"/>
-        <v>0.49820531227566406</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A8" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="3">
-        <v>0</v>
-      </c>
-      <c r="D8" s="3">
-        <v>0.21199999999999999</v>
-      </c>
-      <c r="E8" s="3">
-        <v>0.22700000000000001</v>
-      </c>
-      <c r="F8" s="4">
-        <f t="shared" si="0"/>
-        <v>0.439</v>
-      </c>
-      <c r="G8" s="5">
-        <f t="shared" si="1"/>
-        <v>0.48291571753986329</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A9" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="3">
-        <v>0</v>
-      </c>
-      <c r="D9" s="3">
-        <v>0.83299999999999996</v>
-      </c>
-      <c r="E9" s="3">
-        <v>0.84799999999999998</v>
-      </c>
-      <c r="F9" s="4">
-        <f t="shared" si="0"/>
-        <v>1.681</v>
-      </c>
-      <c r="G9" s="5">
-        <f t="shared" si="1"/>
-        <v>0.49553837001784651</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A10" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="3">
-        <v>0</v>
-      </c>
-      <c r="D10" s="3">
-        <v>1.784</v>
-      </c>
-      <c r="E10" s="3">
-        <v>1.804</v>
-      </c>
-      <c r="F10" s="4">
-        <f t="shared" si="0"/>
-        <v>3.5880000000000001</v>
-      </c>
-      <c r="G10" s="5">
-        <f t="shared" si="1"/>
-        <v>0.49721293199554067</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A11" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="3">
-        <v>1E-3</v>
-      </c>
-      <c r="D11" s="3">
-        <v>0.92800000000000005</v>
-      </c>
-      <c r="E11" s="3">
-        <v>0.99399999999999999</v>
-      </c>
-      <c r="F11" s="4">
-        <f t="shared" si="0"/>
-        <v>1.923</v>
-      </c>
-      <c r="G11" s="5">
-        <f t="shared" si="1"/>
-        <v>0.48257930317212688</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A12" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="3">
-        <v>0</v>
-      </c>
-      <c r="D12" s="3">
-        <v>4.4590000999999999</v>
-      </c>
-      <c r="E12" s="3">
-        <v>4.5500002000000004</v>
-      </c>
-      <c r="F12" s="4">
-        <f t="shared" si="0"/>
-        <v>9.0090003000000003</v>
-      </c>
-      <c r="G12" s="5">
-        <f t="shared" si="1"/>
-        <v>0.49494948956767154</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A13" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="3">
-        <v>0</v>
-      </c>
-      <c r="D13" s="3">
-        <v>8.5939999</v>
-      </c>
-      <c r="E13" s="3">
-        <v>8.6649999999999991</v>
-      </c>
-      <c r="F13" s="4">
-        <f t="shared" si="0"/>
-        <v>17.258999899999999</v>
-      </c>
-      <c r="G13" s="5">
-        <f t="shared" si="1"/>
-        <v>0.49794309924064606</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A14" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="3">
-        <v>0</v>
-      </c>
-      <c r="D14" s="3">
-        <v>2.04</v>
-      </c>
-      <c r="E14" s="3">
-        <v>2.2170000000000001</v>
-      </c>
-      <c r="F14" s="4">
-        <f t="shared" si="0"/>
-        <v>4.2569999999999997</v>
-      </c>
-      <c r="G14" s="5">
-        <f t="shared" si="1"/>
-        <v>0.47921071176885133</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A15" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="3">
-        <v>0</v>
-      </c>
-      <c r="D15" s="3">
-        <v>8.9130000999999996</v>
-      </c>
-      <c r="E15" s="3">
-        <v>9.0979995999999996</v>
-      </c>
-      <c r="F15" s="4">
-        <f t="shared" si="0"/>
-        <v>18.010999699999999</v>
-      </c>
-      <c r="G15" s="5">
-        <f t="shared" si="1"/>
-        <v>0.4948642634200921</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A16" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="3">
-        <v>0</v>
-      </c>
-      <c r="D16" s="3">
-        <v>17.600000399999999</v>
-      </c>
-      <c r="E16" s="3">
-        <v>17.8649998</v>
-      </c>
-      <c r="F16" s="4">
-        <f t="shared" si="0"/>
-        <v>35.465000199999999</v>
-      </c>
-      <c r="G16" s="5">
-        <f t="shared" si="1"/>
-        <v>0.49626393065690722</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A17" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="3">
-        <v>0</v>
-      </c>
-      <c r="D17" s="3">
-        <v>10.574000399999999</v>
-      </c>
-      <c r="E17" s="3">
-        <v>11.689000099999999</v>
-      </c>
-      <c r="F17" s="4">
-        <f t="shared" si="0"/>
-        <v>22.263000499999997</v>
-      </c>
-      <c r="G17" s="5">
-        <f t="shared" si="1"/>
-        <v>0.47495845854201013</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A18" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" s="3">
-        <v>0</v>
-      </c>
-      <c r="D18" s="3">
-        <v>54.3390007</v>
-      </c>
-      <c r="E18" s="3">
-        <v>55.926998099999999</v>
-      </c>
-      <c r="F18" s="4">
-        <f t="shared" si="0"/>
-        <v>110.26599880000001</v>
-      </c>
-      <c r="G18" s="5">
-        <f t="shared" si="1"/>
-        <v>0.49279924266191832</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A19" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C19" s="3">
-        <v>0</v>
-      </c>
-      <c r="D19" s="3">
-        <v>90.435997</v>
-      </c>
-      <c r="E19" s="3">
-        <v>91.883003200000005</v>
-      </c>
-      <c r="F19" s="4">
-        <f t="shared" si="0"/>
-        <v>182.3190002</v>
-      </c>
-      <c r="G19" s="5">
-        <f t="shared" si="1"/>
-        <v>0.49603166373660268</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="18" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
@@ -1665,24 +1227,24 @@
         <v>23</v>
       </c>
       <c r="C2" s="3">
-        <v>0</v>
+        <v>5.3559999999999997E-3</v>
       </c>
       <c r="D2" s="3">
-        <v>1.2E-2</v>
+        <v>8.83E-4</v>
       </c>
       <c r="E2" s="3">
-        <v>1.6E-2</v>
+        <v>1.2719999999999999E-3</v>
       </c>
       <c r="F2" s="3">
-        <v>0.02</v>
+        <v>7.2649999999999998E-3</v>
       </c>
       <c r="G2" s="3">
-        <f>SUM(C2:F2)</f>
-        <v>4.8000000000000001E-2</v>
+        <f>SUM(C2,D2,E2,F2)</f>
+        <v>1.4775999999999999E-2</v>
       </c>
       <c r="H2" s="5">
         <f>E2/G2</f>
-        <v>0.33333333333333331</v>
+        <v>8.6085544125609093E-2</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.4">
@@ -1693,24 +1255,24 @@
         <v>4</v>
       </c>
       <c r="C3" s="3">
-        <v>0</v>
+        <v>2.6362E-2</v>
       </c>
       <c r="D3" s="3">
-        <v>4.3999999999999997E-2</v>
+        <v>4.078E-3</v>
       </c>
       <c r="E3" s="3">
-        <v>5.0999999999999997E-2</v>
+        <v>1.2340000000000001E-3</v>
       </c>
       <c r="F3" s="3">
-        <v>5.6000000000000001E-2</v>
+        <v>2.5037E-2</v>
       </c>
       <c r="G3" s="3">
-        <f t="shared" ref="G3:G19" si="0">SUM(C3:F3)</f>
-        <v>0.151</v>
+        <f t="shared" ref="G3:G18" si="0">SUM(C3,D3,E3,F3)</f>
+        <v>5.6710999999999998E-2</v>
       </c>
       <c r="H3" s="5">
         <f t="shared" ref="H3:H19" si="1">E3/G3</f>
-        <v>0.33774834437086093</v>
+        <v>2.1759447020860152E-2</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.4">
@@ -1721,24 +1283,24 @@
         <v>5</v>
       </c>
       <c r="C4" s="3">
-        <v>0</v>
+        <v>5.2693999999999998E-2</v>
       </c>
       <c r="D4" s="3">
-        <v>0.13400000000000001</v>
+        <v>7.4520000000000003E-3</v>
       </c>
       <c r="E4" s="3">
-        <v>0.14799999999999999</v>
+        <v>1.2470000000000001E-3</v>
       </c>
       <c r="F4" s="3">
-        <v>0.16</v>
+        <v>4.8298000000000001E-2</v>
       </c>
       <c r="G4" s="3">
         <f t="shared" si="0"/>
-        <v>0.44200000000000006</v>
+        <v>0.109691</v>
       </c>
       <c r="H4" s="5">
         <f t="shared" si="1"/>
-        <v>0.33484162895927594</v>
+        <v>1.1368298219543993E-2</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.4">
@@ -1749,24 +1311,24 @@
         <v>6</v>
       </c>
       <c r="C5" s="3">
-        <v>0</v>
+        <v>2.6636E-2</v>
       </c>
       <c r="D5" s="3">
-        <v>5.6000000000000001E-2</v>
+        <v>4.4739999999999997E-3</v>
       </c>
       <c r="E5" s="3">
-        <v>6.2E-2</v>
+        <v>7.711E-3</v>
       </c>
       <c r="F5" s="3">
-        <v>7.1999999999999995E-2</v>
+        <v>3.7554999999999998E-2</v>
       </c>
       <c r="G5" s="3">
         <f t="shared" si="0"/>
-        <v>0.19</v>
+        <v>7.6375999999999999E-2</v>
       </c>
       <c r="H5" s="5">
         <f t="shared" si="1"/>
-        <v>0.32631578947368423</v>
+        <v>0.10096103488006704</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.4">
@@ -1777,24 +1339,24 @@
         <v>7</v>
       </c>
       <c r="C6" s="3">
-        <v>0</v>
+        <v>0.134768</v>
       </c>
       <c r="D6" s="3">
-        <v>0.245</v>
+        <v>1.8956000000000001E-2</v>
       </c>
       <c r="E6" s="3">
-        <v>0.26400000000000001</v>
+        <v>7.7980000000000002E-3</v>
       </c>
       <c r="F6" s="3">
-        <v>0.27400000000000002</v>
+        <v>0.12962599999999999</v>
       </c>
       <c r="G6" s="3">
         <f t="shared" si="0"/>
-        <v>0.78300000000000003</v>
+        <v>0.29114799999999996</v>
       </c>
       <c r="H6" s="5">
         <f t="shared" si="1"/>
-        <v>0.33716475095785442</v>
+        <v>2.6783628944729146E-2</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.4">
@@ -1805,24 +1367,24 @@
         <v>8</v>
       </c>
       <c r="C7" s="3">
-        <v>0</v>
+        <v>0.26546599999999998</v>
       </c>
       <c r="D7" s="3">
-        <v>0.41299999999999998</v>
+        <v>3.7414000000000003E-2</v>
       </c>
       <c r="E7" s="3">
-        <v>0.44700000000000001</v>
+        <v>7.8040000000000002E-3</v>
       </c>
       <c r="F7" s="3">
-        <v>0.45600000000000002</v>
+        <v>0.238983</v>
       </c>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
-        <v>1.3160000000000001</v>
+        <v>0.54966699999999991</v>
       </c>
       <c r="H7" s="5">
         <f t="shared" si="1"/>
-        <v>0.3396656534954407</v>
+        <v>1.4197686963197721E-2</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.4">
@@ -1833,24 +1395,24 @@
         <v>9</v>
       </c>
       <c r="C8" s="3">
-        <v>0</v>
+        <v>5.2956000000000003E-2</v>
       </c>
       <c r="D8" s="3">
-        <v>8.7999999999999995E-2</v>
+        <v>9.0620000000000006E-3</v>
       </c>
       <c r="E8" s="3">
-        <v>9.9000000000000005E-2</v>
+        <v>1.669E-2</v>
       </c>
       <c r="F8" s="3">
-        <v>0.115</v>
+        <v>7.0704000000000003E-2</v>
       </c>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
-        <v>0.30199999999999999</v>
+        <v>0.14941199999999999</v>
       </c>
       <c r="H8" s="5">
         <f t="shared" si="1"/>
-        <v>0.32781456953642385</v>
+        <v>0.11170454849677403</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.4">
@@ -1861,24 +1423,24 @@
         <v>10</v>
       </c>
       <c r="C9" s="3">
-        <v>0</v>
+        <v>0.26478800000000002</v>
       </c>
       <c r="D9" s="3">
-        <v>0.434</v>
+        <v>3.8129999999999997E-2</v>
       </c>
       <c r="E9" s="3">
-        <v>0.47499999999999998</v>
+        <v>1.7170000000000001E-2</v>
       </c>
       <c r="F9" s="3">
-        <v>0.504</v>
+        <v>0.25917299999999999</v>
       </c>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
-        <v>1.413</v>
+        <v>0.57926100000000003</v>
       </c>
       <c r="H9" s="5">
         <f t="shared" si="1"/>
-        <v>0.33616418966737438</v>
+        <v>2.9641215272562801E-2</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.4">
@@ -1889,24 +1451,24 @@
         <v>11</v>
       </c>
       <c r="C10" s="3">
-        <v>0</v>
+        <v>0.53488400000000003</v>
       </c>
       <c r="D10" s="3">
-        <v>0.84599999999999997</v>
+        <v>7.6501E-2</v>
       </c>
       <c r="E10" s="3">
-        <v>0.91</v>
+        <v>1.7821E-2</v>
       </c>
       <c r="F10" s="3">
-        <v>0.92700000000000005</v>
+        <v>0.483435</v>
       </c>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
-        <v>2.6829999999999998</v>
+        <v>1.112641</v>
       </c>
       <c r="H10" s="5">
         <f t="shared" si="1"/>
-        <v>0.3391725680208722</v>
+        <v>1.6016846404186075E-2</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.4">
@@ -1917,24 +1479,24 @@
         <v>12</v>
       </c>
       <c r="C11" s="3">
-        <v>0</v>
+        <v>0.26855200000000001</v>
       </c>
       <c r="D11" s="3">
-        <v>0.435</v>
+        <v>4.4739000000000001E-2</v>
       </c>
       <c r="E11" s="3">
-        <v>0.48099999999999998</v>
+        <v>0.101729</v>
       </c>
       <c r="F11" s="3">
-        <v>0.57399999999999995</v>
+        <v>0.387353</v>
       </c>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
-        <v>1.4899999999999998</v>
+        <v>0.802373</v>
       </c>
       <c r="H11" s="5">
         <f t="shared" si="1"/>
-        <v>0.32281879194630875</v>
+        <v>0.12678517347916743</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.4">
@@ -1945,24 +1507,24 @@
         <v>13</v>
       </c>
       <c r="C12" s="3">
-        <v>0</v>
+        <v>1.3266701000000001</v>
       </c>
       <c r="D12" s="3">
-        <v>2.4170001000000001</v>
+        <v>0.18992100000000001</v>
       </c>
       <c r="E12" s="3">
-        <v>2.5969999000000001</v>
+        <v>0.106777</v>
       </c>
       <c r="F12" s="3">
-        <v>2.7109999999999999</v>
+        <v>1.3036391000000001</v>
       </c>
       <c r="G12" s="3">
         <f t="shared" si="0"/>
-        <v>7.7249999999999996</v>
+        <v>2.9270072000000003</v>
       </c>
       <c r="H12" s="5">
         <f t="shared" si="1"/>
-        <v>0.33618121682847901</v>
+        <v>3.6479923930491182E-2</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.4">
@@ -1973,24 +1535,24 @@
         <v>14</v>
       </c>
       <c r="C13" s="3">
-        <v>0</v>
+        <v>2.6492870000000002</v>
       </c>
       <c r="D13" s="3">
-        <v>5.4330001000000001</v>
+        <v>0.37345299999999998</v>
       </c>
       <c r="E13" s="3">
-        <v>5.7820001000000003</v>
+        <v>0.109349</v>
       </c>
       <c r="F13" s="3">
-        <v>5.8860001999999998</v>
+        <v>2.4067210999999999</v>
       </c>
       <c r="G13" s="3">
         <f t="shared" si="0"/>
-        <v>17.1010004</v>
+        <v>5.5388101000000001</v>
       </c>
       <c r="H13" s="5">
         <f t="shared" si="1"/>
-        <v>0.33810888046058407</v>
+        <v>1.9742326966580782E-2</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.4">
@@ -2001,24 +1563,24 @@
         <v>15</v>
       </c>
       <c r="C14" s="3">
-        <v>0</v>
+        <v>0.53346099999999996</v>
       </c>
       <c r="D14" s="3">
-        <v>0.876</v>
+        <v>8.9342000000000005E-2</v>
       </c>
       <c r="E14" s="3">
-        <v>0.998</v>
+        <v>0.22936899999999999</v>
       </c>
       <c r="F14" s="3">
-        <v>1.395</v>
+        <v>0.80263899999999999</v>
       </c>
       <c r="G14" s="3">
         <f t="shared" si="0"/>
-        <v>3.2690000000000001</v>
+        <v>1.654811</v>
       </c>
       <c r="H14" s="5">
         <f t="shared" si="1"/>
-        <v>0.30529213826858365</v>
+        <v>0.13860736966336337</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.4">
@@ -2029,24 +1591,24 @@
         <v>16</v>
       </c>
       <c r="C15" s="3">
-        <v>0</v>
+        <v>2.6397409000000001</v>
       </c>
       <c r="D15" s="3">
-        <v>5.2729998</v>
+        <v>0.379025</v>
       </c>
       <c r="E15" s="3">
-        <v>5.6339997999999998</v>
+        <v>0.24101</v>
       </c>
       <c r="F15" s="3">
-        <v>5.8689999999999998</v>
+        <v>2.6153431</v>
       </c>
       <c r="G15" s="3">
         <f t="shared" si="0"/>
-        <v>16.775999599999999</v>
+        <v>5.8751189999999998</v>
       </c>
       <c r="H15" s="5">
         <f t="shared" si="1"/>
-        <v>0.33583690595700777</v>
+        <v>4.1022147806708258E-2</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.4">
@@ -2057,24 +1619,24 @@
         <v>17</v>
       </c>
       <c r="C16" s="3">
-        <v>0</v>
+        <v>5.3402748000000004</v>
       </c>
       <c r="D16" s="3">
-        <v>10.8559999</v>
+        <v>0.74307000000000001</v>
       </c>
       <c r="E16" s="3">
-        <v>11.593000399999999</v>
+        <v>0.246256</v>
       </c>
       <c r="F16" s="3">
-        <v>11.847000100000001</v>
+        <v>4.8353782000000001</v>
       </c>
       <c r="G16" s="3">
         <f t="shared" si="0"/>
-        <v>34.296000400000004</v>
+        <v>11.164979000000001</v>
       </c>
       <c r="H16" s="5">
         <f t="shared" si="1"/>
-        <v>0.33802776605985807</v>
+        <v>2.2056109554706729E-2</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.4">
@@ -2085,24 +1647,24 @@
         <v>18</v>
       </c>
       <c r="C17" s="3">
-        <v>0</v>
+        <v>2.6691940000000001</v>
       </c>
       <c r="D17" s="3">
-        <v>5.3010001000000004</v>
+        <v>0.44449899999999998</v>
       </c>
       <c r="E17" s="3">
-        <v>5.8169998999999999</v>
+        <v>1.3910629999999999</v>
       </c>
       <c r="F17" s="3">
-        <v>7.3070002000000001</v>
+        <v>4.0110469000000002</v>
       </c>
       <c r="G17" s="3">
         <f t="shared" si="0"/>
-        <v>18.425000199999999</v>
+        <v>8.5158029000000006</v>
       </c>
       <c r="H17" s="5">
         <f t="shared" si="1"/>
-        <v>0.3157123384997304</v>
+        <v>0.16335077459343261</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.4">
@@ -2113,24 +1675,24 @@
         <v>19</v>
       </c>
       <c r="C18" s="3">
-        <v>0</v>
+        <v>13.230498300000001</v>
       </c>
       <c r="D18" s="3">
-        <v>26.226999299999999</v>
+        <v>1.900468</v>
       </c>
       <c r="E18" s="3">
-        <v>28.892000199999998</v>
+        <v>1.5172330000000001</v>
       </c>
       <c r="F18" s="3">
-        <v>30.7369995</v>
+        <v>13.100207299999999</v>
       </c>
       <c r="G18" s="3">
         <f t="shared" si="0"/>
-        <v>85.855998999999997</v>
+        <v>29.748406600000003</v>
       </c>
       <c r="H18" s="5">
         <f t="shared" si="1"/>
-        <v>0.33651696487743388</v>
+        <v>5.1002160229986902E-2</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.4">
@@ -2141,24 +1703,519 @@
         <v>20</v>
       </c>
       <c r="C19" s="3">
-        <v>0</v>
+        <v>26.384513900000002</v>
       </c>
       <c r="D19" s="3">
-        <v>49.310001399999997</v>
+        <v>3.7805990999999999</v>
       </c>
       <c r="E19" s="3">
-        <v>52.419998200000002</v>
+        <v>1.5966720999999999</v>
       </c>
       <c r="F19" s="3">
-        <v>53.858001700000003</v>
+        <v>24.401468300000001</v>
       </c>
       <c r="G19" s="3">
-        <f t="shared" si="0"/>
-        <v>155.5880013</v>
+        <f>SUM(C19,D19,E19,F19)</f>
+        <v>56.163253400000002</v>
       </c>
       <c r="H19" s="5">
-        <f t="shared" si="1"/>
-        <v>0.33691542896630811</v>
+        <f>E19/G19</f>
+        <v>2.84291240863194E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G19"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="2" max="2" width="19.1796875" customWidth="1"/>
+    <col min="3" max="3" width="17.36328125" customWidth="1"/>
+    <col min="4" max="4" width="17.6328125" customWidth="1"/>
+    <col min="5" max="5" width="17.36328125" customWidth="1"/>
+    <col min="6" max="6" width="18.6328125" customWidth="1"/>
+    <col min="7" max="7" width="15.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="B1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="3">
+        <v>3.447E-3</v>
+      </c>
+      <c r="D2" s="3">
+        <v>4.15E-4</v>
+      </c>
+      <c r="E2" s="3">
+        <v>3.2799999999999999E-3</v>
+      </c>
+      <c r="F2" s="4">
+        <f>SUM(C2,D2,E2)</f>
+        <v>7.1419999999999999E-3</v>
+      </c>
+      <c r="G2" s="5">
+        <f>D2/F2</f>
+        <v>5.8106972836740413E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1.5918999999999999E-2</v>
+      </c>
+      <c r="D3" s="3">
+        <v>4.4099999999999999E-4</v>
+      </c>
+      <c r="E3" s="3">
+        <v>4.3909999999999999E-3</v>
+      </c>
+      <c r="F3" s="4">
+        <f t="shared" ref="F3:F19" si="0">SUM(C3,D3,E3)</f>
+        <v>2.0750999999999999E-2</v>
+      </c>
+      <c r="G3" s="5">
+        <f t="shared" ref="G3:G19" si="1">D3/F3</f>
+        <v>2.1251987856006939E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="3">
+        <v>3.1525999999999998E-2</v>
+      </c>
+      <c r="D4" s="3">
+        <v>4.37E-4</v>
+      </c>
+      <c r="E4" s="3">
+        <v>6.5620000000000001E-3</v>
+      </c>
+      <c r="F4" s="4">
+        <f t="shared" si="0"/>
+        <v>3.8524999999999997E-2</v>
+      </c>
+      <c r="G4" s="5">
+        <f t="shared" si="1"/>
+        <v>1.1343283582089553E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1.7177999999999999E-2</v>
+      </c>
+      <c r="D5" s="3">
+        <v>2.5439999999999998E-3</v>
+      </c>
+      <c r="E5" s="3">
+        <v>1.5730999999999998E-2</v>
+      </c>
+      <c r="F5" s="4">
+        <f t="shared" si="0"/>
+        <v>3.5452999999999998E-2</v>
+      </c>
+      <c r="G5" s="5">
+        <f t="shared" si="1"/>
+        <v>7.1756974021944545E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="3">
+        <v>7.9655000000000004E-2</v>
+      </c>
+      <c r="D6" s="3">
+        <v>2.8310000000000002E-3</v>
+      </c>
+      <c r="E6" s="3">
+        <v>2.4122000000000001E-2</v>
+      </c>
+      <c r="F6" s="4">
+        <f t="shared" si="0"/>
+        <v>0.10660800000000001</v>
+      </c>
+      <c r="G6" s="5">
+        <f t="shared" si="1"/>
+        <v>2.6555230376707189E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.15687699999999999</v>
+      </c>
+      <c r="D7" s="3">
+        <v>2.905E-3</v>
+      </c>
+      <c r="E7" s="3">
+        <v>3.4164E-2</v>
+      </c>
+      <c r="F7" s="4">
+        <f t="shared" si="0"/>
+        <v>0.19394599999999998</v>
+      </c>
+      <c r="G7" s="5">
+        <f t="shared" si="1"/>
+        <v>1.4978396048384603E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="3">
+        <v>3.4473999999999998E-2</v>
+      </c>
+      <c r="D8" s="3">
+        <v>5.4390000000000003E-3</v>
+      </c>
+      <c r="E8" s="3">
+        <v>2.1651E-2</v>
+      </c>
+      <c r="F8" s="4">
+        <f t="shared" si="0"/>
+        <v>6.1563999999999994E-2</v>
+      </c>
+      <c r="G8" s="5">
+        <f t="shared" si="1"/>
+        <v>8.8347085959326888E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0.16036700000000001</v>
+      </c>
+      <c r="D9" s="3">
+        <v>6.4339999999999996E-3</v>
+      </c>
+      <c r="E9" s="3">
+        <v>4.9482999999999999E-2</v>
+      </c>
+      <c r="F9" s="4">
+        <f t="shared" si="0"/>
+        <v>0.216284</v>
+      </c>
+      <c r="G9" s="5">
+        <f t="shared" si="1"/>
+        <v>2.9747924025817905E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.31784099999999998</v>
+      </c>
+      <c r="D10" s="3">
+        <v>7.0679999999999996E-3</v>
+      </c>
+      <c r="E10" s="3">
+        <v>6.7943000000000003E-2</v>
+      </c>
+      <c r="F10" s="4">
+        <f t="shared" si="0"/>
+        <v>0.39285199999999998</v>
+      </c>
+      <c r="G10" s="5">
+        <f t="shared" si="1"/>
+        <v>1.7991508252471668E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.16958999999999999</v>
+      </c>
+      <c r="D11" s="3">
+        <v>3.6749999999999998E-2</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0.153474</v>
+      </c>
+      <c r="F11" s="4">
+        <f t="shared" si="0"/>
+        <v>0.35981399999999997</v>
+      </c>
+      <c r="G11" s="5">
+        <f t="shared" si="1"/>
+        <v>0.10213610365355434</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0.79625400000000002</v>
+      </c>
+      <c r="D12" s="3">
+        <v>4.1952000000000003E-2</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0.238259</v>
+      </c>
+      <c r="F12" s="4">
+        <f t="shared" si="0"/>
+        <v>1.076465</v>
+      </c>
+      <c r="G12" s="5">
+        <f t="shared" si="1"/>
+        <v>3.8972005592378761E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="3">
+        <v>1.570292</v>
+      </c>
+      <c r="D13" s="3">
+        <v>4.6001E-2</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0.34691499999999997</v>
+      </c>
+      <c r="F13" s="4">
+        <f t="shared" si="0"/>
+        <v>1.9632079999999998</v>
+      </c>
+      <c r="G13" s="5">
+        <f t="shared" si="1"/>
+        <v>2.3431546733713393E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A14" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0.34122000000000002</v>
+      </c>
+      <c r="D14" s="3">
+        <v>7.4773000000000006E-2</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0.22355900000000001</v>
+      </c>
+      <c r="F14" s="4">
+        <f t="shared" si="0"/>
+        <v>0.63955200000000012</v>
+      </c>
+      <c r="G14" s="5">
+        <f t="shared" si="1"/>
+        <v>0.11691465275692983</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A15" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="3">
+        <v>1.6061989999999999</v>
+      </c>
+      <c r="D15" s="3">
+        <v>9.5857999999999999E-2</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0.48579</v>
+      </c>
+      <c r="F15" s="4">
+        <f t="shared" si="0"/>
+        <v>2.1878470000000001</v>
+      </c>
+      <c r="G15" s="5">
+        <f t="shared" si="1"/>
+        <v>4.3813849871586083E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A16" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="3">
+        <v>3.142941</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0.10394399999999999</v>
+      </c>
+      <c r="E16" s="3">
+        <v>0.72036800000000001</v>
+      </c>
+      <c r="F16" s="4">
+        <f t="shared" si="0"/>
+        <v>3.9672529999999999</v>
+      </c>
+      <c r="G16" s="5">
+        <f t="shared" si="1"/>
+        <v>2.620049691814462E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A17" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="3">
+        <v>1.7188848999999999</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0.52555499999999999</v>
+      </c>
+      <c r="E17" s="3">
+        <v>1.3502289999999999</v>
+      </c>
+      <c r="F17" s="4">
+        <f t="shared" si="0"/>
+        <v>3.5946688999999994</v>
+      </c>
+      <c r="G17" s="5">
+        <f t="shared" si="1"/>
+        <v>0.14620400782948328</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A18" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="3">
+        <v>7.9632049</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0.66245200000000004</v>
+      </c>
+      <c r="E18" s="3">
+        <v>2.4552591000000001</v>
+      </c>
+      <c r="F18" s="4">
+        <f t="shared" si="0"/>
+        <v>11.080915999999998</v>
+      </c>
+      <c r="G18" s="5">
+        <f t="shared" si="1"/>
+        <v>5.9783144281573844E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A19" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="3">
+        <v>15.7894497</v>
+      </c>
+      <c r="D19" s="3">
+        <v>0.69860900000000004</v>
+      </c>
+      <c r="E19" s="3">
+        <v>3.5495801</v>
+      </c>
+      <c r="F19" s="4">
+        <f t="shared" si="0"/>
+        <v>20.0376388</v>
+      </c>
+      <c r="G19" s="5">
+        <f t="shared" si="1"/>
+        <v>3.4864836469654298E-2</v>
       </c>
     </row>
   </sheetData>
@@ -2172,8 +2229,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G19"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
@@ -2214,21 +2271,21 @@
         <v>3</v>
       </c>
       <c r="C2" s="3">
-        <v>0</v>
+        <v>3.3479999999999998E-3</v>
       </c>
       <c r="D2" s="3">
-        <v>1.9E-2</v>
+        <v>3.9500000000000001E-4</v>
       </c>
       <c r="E2" s="3">
-        <v>2.5999999999999999E-2</v>
+        <v>2.66E-3</v>
       </c>
       <c r="F2" s="4">
-        <f>SUM(C2:E2)</f>
-        <v>4.4999999999999998E-2</v>
+        <f>SUM(C2,D2,E2)</f>
+        <v>6.4029999999999998E-3</v>
       </c>
       <c r="G2" s="5">
         <f>D2/F2</f>
-        <v>0.42222222222222222</v>
+        <v>6.1689832890832422E-2</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.4">
@@ -2239,21 +2296,21 @@
         <v>4</v>
       </c>
       <c r="C3" s="3">
-        <v>0</v>
+        <v>1.5795E-2</v>
       </c>
       <c r="D3" s="3">
-        <v>0.08</v>
+        <v>5.1099999999999995E-4</v>
       </c>
       <c r="E3" s="3">
-        <v>8.8999999999999996E-2</v>
+        <v>4.705E-3</v>
       </c>
       <c r="F3" s="4">
-        <f t="shared" ref="F3:F19" si="0">SUM(C3:E3)</f>
-        <v>0.16899999999999998</v>
+        <f t="shared" ref="F3:F19" si="0">SUM(C3,D3,E3)</f>
+        <v>2.1011000000000002E-2</v>
       </c>
       <c r="G3" s="5">
         <f t="shared" ref="G3:G19" si="1">D3/F3</f>
-        <v>0.47337278106508879</v>
+        <v>2.4320593974584737E-2</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.4">
@@ -2264,21 +2321,21 @@
         <v>5</v>
       </c>
       <c r="C4" s="3">
-        <v>0</v>
+        <v>3.1616999999999999E-2</v>
       </c>
       <c r="D4" s="3">
-        <v>0.185</v>
+        <v>4.28E-4</v>
       </c>
       <c r="E4" s="3">
-        <v>0.191</v>
+        <v>9.0919999999999994E-3</v>
       </c>
       <c r="F4" s="4">
         <f t="shared" si="0"/>
-        <v>0.376</v>
+        <v>4.1136999999999993E-2</v>
       </c>
       <c r="G4" s="5">
         <f t="shared" si="1"/>
-        <v>0.49202127659574468</v>
+        <v>1.0404258939640714E-2</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.4">
@@ -2289,21 +2346,21 @@
         <v>6</v>
       </c>
       <c r="C5" s="3">
-        <v>0</v>
+        <v>1.7124E-2</v>
       </c>
       <c r="D5" s="3">
-        <v>0.11799999999999999</v>
+        <v>2.5330000000000001E-3</v>
       </c>
       <c r="E5" s="3">
-        <v>0.13600000000000001</v>
+        <v>1.5802E-2</v>
       </c>
       <c r="F5" s="4">
         <f t="shared" si="0"/>
-        <v>0.254</v>
+        <v>3.5459000000000004E-2</v>
       </c>
       <c r="G5" s="5">
         <f t="shared" si="1"/>
-        <v>0.46456692913385822</v>
+        <v>7.1434614625341938E-2</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.4">
@@ -2314,21 +2371,21 @@
         <v>7</v>
       </c>
       <c r="C6" s="3">
-        <v>0</v>
+        <v>8.0631999999999995E-2</v>
       </c>
       <c r="D6" s="3">
-        <v>0.48399999999999999</v>
+        <v>2.712E-3</v>
       </c>
       <c r="E6" s="3">
-        <v>0.496</v>
+        <v>2.2145000000000001E-2</v>
       </c>
       <c r="F6" s="4">
         <f t="shared" si="0"/>
-        <v>0.98</v>
+        <v>0.105489</v>
       </c>
       <c r="G6" s="5">
         <f t="shared" si="1"/>
-        <v>0.49387755102040815</v>
+        <v>2.5708841680175183E-2</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.4">
@@ -2339,21 +2396,21 @@
         <v>8</v>
       </c>
       <c r="C7" s="3">
-        <v>0</v>
+        <v>0.161222</v>
       </c>
       <c r="D7" s="3">
-        <v>1.2250000000000001</v>
+        <v>2.931E-3</v>
       </c>
       <c r="E7" s="3">
-        <v>1.24</v>
+        <v>3.3575000000000001E-2</v>
       </c>
       <c r="F7" s="4">
         <f t="shared" si="0"/>
-        <v>2.4649999999999999</v>
+        <v>0.19772799999999999</v>
       </c>
       <c r="G7" s="5">
         <f t="shared" si="1"/>
-        <v>0.49695740365111568</v>
+        <v>1.4823393753034472E-2</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.4">
@@ -2364,21 +2421,21 @@
         <v>9</v>
       </c>
       <c r="C8" s="3">
-        <v>0</v>
+        <v>3.3516999999999998E-2</v>
       </c>
       <c r="D8" s="3">
-        <v>0.21199999999999999</v>
+        <v>5.3169999999999997E-3</v>
       </c>
       <c r="E8" s="3">
-        <v>0.22800000000000001</v>
+        <v>2.2738000000000001E-2</v>
       </c>
       <c r="F8" s="4">
         <f t="shared" si="0"/>
-        <v>0.44</v>
+        <v>6.1572000000000002E-2</v>
       </c>
       <c r="G8" s="5">
         <f t="shared" si="1"/>
-        <v>0.48181818181818181</v>
+        <v>8.6354186968102375E-2</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.4">
@@ -2389,21 +2446,21 @@
         <v>10</v>
       </c>
       <c r="C9" s="3">
-        <v>0</v>
+        <v>0.157304</v>
       </c>
       <c r="D9" s="3">
-        <v>0.754</v>
+        <v>6.1139999999999996E-3</v>
       </c>
       <c r="E9" s="3">
-        <v>0.77200000000000002</v>
+        <v>4.4005000000000002E-2</v>
       </c>
       <c r="F9" s="4">
         <f t="shared" si="0"/>
-        <v>1.526</v>
+        <v>0.20742300000000002</v>
       </c>
       <c r="G9" s="5">
         <f t="shared" si="1"/>
-        <v>0.49410222804718218</v>
+        <v>2.9475998322268982E-2</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.4">
@@ -2414,21 +2471,21 @@
         <v>11</v>
       </c>
       <c r="C10" s="3">
-        <v>0</v>
+        <v>0.31540699999999999</v>
       </c>
       <c r="D10" s="3">
-        <v>1.863</v>
+        <v>6.4320000000000002E-3</v>
       </c>
       <c r="E10" s="3">
-        <v>1.89</v>
+        <v>6.8793999999999994E-2</v>
       </c>
       <c r="F10" s="4">
         <f t="shared" si="0"/>
-        <v>3.7530000000000001</v>
+        <v>0.39063300000000001</v>
       </c>
       <c r="G10" s="5">
         <f t="shared" si="1"/>
-        <v>0.49640287769784169</v>
+        <v>1.6465582784864565E-2</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.4">
@@ -2439,21 +2496,21 @@
         <v>12</v>
       </c>
       <c r="C11" s="3">
-        <v>0</v>
+        <v>0.16877300000000001</v>
       </c>
       <c r="D11" s="3">
-        <v>0.76300000000000001</v>
+        <v>3.3862000000000003E-2</v>
       </c>
       <c r="E11" s="3">
-        <v>0.82099999999999995</v>
+        <v>0.13764799999999999</v>
       </c>
       <c r="F11" s="4">
         <f t="shared" si="0"/>
-        <v>1.5840000000000001</v>
+        <v>0.340283</v>
       </c>
       <c r="G11" s="5">
         <f t="shared" si="1"/>
-        <v>0.48169191919191917</v>
+        <v>9.951128913286883E-2</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.4">
@@ -2464,21 +2521,21 @@
         <v>13</v>
       </c>
       <c r="C12" s="3">
-        <v>0</v>
+        <v>0.79109499999999999</v>
       </c>
       <c r="D12" s="3">
-        <v>4.3600000999999997</v>
+        <v>4.3570999999999999E-2</v>
       </c>
       <c r="E12" s="3">
-        <v>4.4489998999999996</v>
+        <v>0.24380499999999999</v>
       </c>
       <c r="F12" s="4">
         <f t="shared" si="0"/>
-        <v>8.8089999999999993</v>
+        <v>1.078471</v>
       </c>
       <c r="G12" s="5">
         <f t="shared" si="1"/>
-        <v>0.49494835963219436</v>
+        <v>4.040071545734656E-2</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.4">
@@ -2489,21 +2546,21 @@
         <v>14</v>
       </c>
       <c r="C13" s="3">
-        <v>0</v>
+        <v>1.571774</v>
       </c>
       <c r="D13" s="3">
-        <v>7.1030002000000003</v>
+        <v>4.6580999999999997E-2</v>
       </c>
       <c r="E13" s="3">
-        <v>7.1890001000000003</v>
+        <v>0.34473500000000001</v>
       </c>
       <c r="F13" s="4">
         <f t="shared" si="0"/>
-        <v>14.292000300000002</v>
+        <v>1.96309</v>
       </c>
       <c r="G13" s="5">
         <f t="shared" si="1"/>
-        <v>0.49699132737913526</v>
+        <v>2.3728407765308771E-2</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.4">
@@ -2514,21 +2571,21 @@
         <v>15</v>
       </c>
       <c r="C14" s="3">
-        <v>0</v>
+        <v>0.33610099999999998</v>
       </c>
       <c r="D14" s="3">
-        <v>1.7640001000000001</v>
+        <v>7.7974000000000002E-2</v>
       </c>
       <c r="E14" s="3">
-        <v>1.903</v>
+        <v>0.31237799999999999</v>
       </c>
       <c r="F14" s="4">
         <f t="shared" si="0"/>
-        <v>3.6670001000000001</v>
+        <v>0.72645300000000002</v>
       </c>
       <c r="G14" s="5">
         <f t="shared" si="1"/>
-        <v>0.4810471916812874</v>
+        <v>0.10733523022136325</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.4">
@@ -2539,21 +2596,21 @@
         <v>16</v>
       </c>
       <c r="C15" s="3">
-        <v>0</v>
+        <v>1.5775140999999999</v>
       </c>
       <c r="D15" s="3">
-        <v>8.4420003999999995</v>
+        <v>0.100226</v>
       </c>
       <c r="E15" s="3">
-        <v>8.5939999</v>
+        <v>0.48255900000000002</v>
       </c>
       <c r="F15" s="4">
         <f t="shared" si="0"/>
-        <v>17.036000299999998</v>
+        <v>2.1602991</v>
       </c>
       <c r="G15" s="5">
         <f t="shared" si="1"/>
-        <v>0.49553887364042842</v>
+        <v>4.6394501576193778E-2</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.4">
@@ -2564,21 +2621,21 @@
         <v>17</v>
       </c>
       <c r="C16" s="3">
-        <v>0</v>
+        <v>3.2841520000000002</v>
       </c>
       <c r="D16" s="3">
-        <v>20.415000899999999</v>
+        <v>0.11025600000000001</v>
       </c>
       <c r="E16" s="3">
-        <v>20.621000299999999</v>
+        <v>0.69542199999999998</v>
       </c>
       <c r="F16" s="4">
         <f t="shared" si="0"/>
-        <v>41.036001200000001</v>
+        <v>4.0898300000000001</v>
       </c>
       <c r="G16" s="5">
         <f t="shared" si="1"/>
-        <v>0.49749001615683741</v>
+        <v>2.695857774039508E-2</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.4">
@@ -2589,21 +2646,21 @@
         <v>18</v>
       </c>
       <c r="C17" s="3">
-        <v>0</v>
+        <v>1.6619950999999999</v>
       </c>
       <c r="D17" s="3">
-        <v>9.6789999000000009</v>
+        <v>0.51688000000000001</v>
       </c>
       <c r="E17" s="3">
-        <v>10.8269997</v>
+        <v>1.468791</v>
       </c>
       <c r="F17" s="4">
         <f t="shared" si="0"/>
-        <v>20.505999600000003</v>
+        <v>3.6476660999999999</v>
       </c>
       <c r="G17" s="5">
         <f t="shared" si="1"/>
-        <v>0.4720081970546805</v>
+        <v>0.14170156637966397</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.4">
@@ -2614,21 +2671,21 @@
         <v>19</v>
       </c>
       <c r="C18" s="3">
-        <v>0</v>
+        <v>7.9472842000000004</v>
       </c>
       <c r="D18" s="3">
-        <v>44.9679985</v>
+        <v>0.64896600000000004</v>
       </c>
       <c r="E18" s="3">
-        <v>46.381000499999999</v>
+        <v>2.5276529999999999</v>
       </c>
       <c r="F18" s="4">
         <f t="shared" si="0"/>
-        <v>91.348998999999992</v>
+        <v>11.123903200000001</v>
       </c>
       <c r="G18" s="5">
         <f t="shared" si="1"/>
-        <v>0.49226591415632265</v>
+        <v>5.8339774118135082E-2</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.4">
@@ -2639,21 +2696,1204 @@
         <v>20</v>
       </c>
       <c r="C19" s="3">
-        <v>0</v>
+        <v>15.7425642</v>
       </c>
       <c r="D19" s="3">
-        <v>93.619003300000003</v>
+        <v>0.68350900000000003</v>
       </c>
       <c r="E19" s="3">
-        <v>94.877998399999996</v>
+        <v>3.6153960000000001</v>
       </c>
       <c r="F19" s="4">
         <f t="shared" si="0"/>
-        <v>188.4970017</v>
+        <v>20.041469200000002</v>
       </c>
       <c r="G19" s="5">
         <f t="shared" si="1"/>
-        <v>0.496660437331508</v>
+        <v>3.4104735195760995E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H19"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:F19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="2" max="2" width="22.7265625" customWidth="1"/>
+    <col min="3" max="3" width="17.36328125" customWidth="1"/>
+    <col min="4" max="4" width="25.08984375" customWidth="1"/>
+    <col min="5" max="5" width="23.54296875" customWidth="1"/>
+    <col min="6" max="6" width="19.1796875" customWidth="1"/>
+    <col min="7" max="7" width="17.453125" customWidth="1"/>
+    <col min="8" max="8" width="17.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="B1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3">
+        <f>SUM(C2,D2,E2,F2)</f>
+        <v>0</v>
+      </c>
+      <c r="H2" s="5" t="e">
+        <f>E2/G2</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3">
+        <f t="shared" ref="G3:G18" si="0">SUM(C3,D3,E3,F3)</f>
+        <v>0</v>
+      </c>
+      <c r="H3" s="5" t="e">
+        <f t="shared" ref="H3:H19" si="1">E3/G3</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H4" s="5" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H5" s="5" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H6" s="5" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H7" s="5" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H8" s="5" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H9" s="5" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H10" s="5" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H11" s="5" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H12" s="5" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H13" s="5" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A14" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H14" s="5" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A15" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H15" s="5" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A16" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H16" s="5" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A17" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H17" s="5" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A18" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H18" s="5" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A19" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3">
+        <f>SUM(C19,D19,E19,F19)</f>
+        <v>0</v>
+      </c>
+      <c r="H19" s="5" t="e">
+        <f>E19/G19</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:E19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="2" max="2" width="19.1796875" customWidth="1"/>
+    <col min="3" max="3" width="17.36328125" customWidth="1"/>
+    <col min="4" max="4" width="17.6328125" customWidth="1"/>
+    <col min="5" max="5" width="17.36328125" customWidth="1"/>
+    <col min="6" max="6" width="18.6328125" customWidth="1"/>
+    <col min="7" max="7" width="15.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="B1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="4">
+        <f>SUM(C2,D2,E2)</f>
+        <v>0</v>
+      </c>
+      <c r="G2" s="5" t="e">
+        <f>D2/F2</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="4">
+        <f t="shared" ref="F3:F19" si="0">SUM(C3,D3,E3)</f>
+        <v>0</v>
+      </c>
+      <c r="G3" s="5" t="e">
+        <f t="shared" ref="G3:G19" si="1">D3/F3</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G4" s="5" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G5" s="5" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G6" s="5" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G7" s="5" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G8" s="5" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G9" s="5" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G10" s="5" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G11" s="5" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G12" s="5" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G13" s="5" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A14" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G14" s="5" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A15" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G15" s="5" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A16" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G16" s="5" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A17" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G17" s="5" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A18" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G18" s="5" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A19" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G19" s="5" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="2" max="2" width="19.1796875" customWidth="1"/>
+    <col min="3" max="3" width="17.36328125" customWidth="1"/>
+    <col min="4" max="4" width="17.6328125" customWidth="1"/>
+    <col min="5" max="5" width="17.36328125" customWidth="1"/>
+    <col min="6" max="6" width="19.54296875" customWidth="1"/>
+    <col min="7" max="7" width="17.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="4">
+        <f>SUM(C2,D2,E2)</f>
+        <v>0</v>
+      </c>
+      <c r="G2" s="5" t="e">
+        <f>D2/F2</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="4">
+        <f t="shared" ref="F3:F19" si="0">SUM(C3,D3,E3)</f>
+        <v>0</v>
+      </c>
+      <c r="G3" s="5" t="e">
+        <f t="shared" ref="G3:G19" si="1">D3/F3</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G4" s="5" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G5" s="5" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G6" s="5" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G7" s="5" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G8" s="5" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G9" s="5" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G10" s="5" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G11" s="5" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G12" s="5" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G13" s="5" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A14" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G14" s="5" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A15" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G15" s="5" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A16" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G16" s="5" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A17" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G17" s="5" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A18" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G18" s="5" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A19" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G19" s="5" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>